<commit_message>
improve gpio bit arrangement
</commit_message>
<xml_diff>
--- a/design/gpio-bit-arrangement.xlsx
+++ b/design/gpio-bit-arrangement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="2580" windowWidth="25600" windowHeight="18600" tabRatio="500"/>
+    <workbookView xWindow="6440" yWindow="1080" windowWidth="21440" windowHeight="21920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="5">
   <si>
     <t>GND</t>
   </si>
@@ -27,22 +27,13 @@
     <t>GPIO Bit</t>
   </si>
   <si>
-    <r>
-      <t>NN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>=Logic Analyzer Only</t>
-    </r>
-  </si>
-  <si>
     <t>JXn</t>
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>preferred</t>
   </si>
 </sst>
 </file>
@@ -105,7 +96,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +139,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -173,7 +194,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -215,8 +236,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -276,8 +299,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -298,6 +343,7 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -318,6 +364,7 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -647,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -660,24 +707,38 @@
     <col min="3" max="3" width="3.6640625" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" style="14" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="15" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="13"/>
+    <col min="6" max="6" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:9">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="20"/>
       <c r="D1" s="12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="20"/>
+      <c r="I1" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -685,13 +746,21 @@
       <c r="C2" s="3">
         <v>2</v>
       </c>
-      <c r="D2" s="16">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2" s="16"/>
+      <c r="F2" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3">
+        <v>2</v>
+      </c>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
@@ -699,12 +768,24 @@
       <c r="C3" s="4">
         <v>4</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="21">
+        <v>24</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2">
+        <v>3</v>
+      </c>
+      <c r="H3" s="4">
+        <v>4</v>
+      </c>
+      <c r="I3" s="21">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="17">
+    <row r="4" spans="1:9">
+      <c r="A4" s="25">
         <v>8</v>
       </c>
       <c r="B4" s="6">
@@ -713,12 +794,24 @@
       <c r="C4" s="7">
         <v>6</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="22">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="17">
+      <c r="F4" s="25">
+        <v>8</v>
+      </c>
+      <c r="G4" s="6">
+        <v>5</v>
+      </c>
+      <c r="H4" s="7">
+        <v>6</v>
+      </c>
+      <c r="I4" s="22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="25">
         <v>9</v>
       </c>
       <c r="B5" s="7">
@@ -727,11 +820,23 @@
       <c r="C5" s="6">
         <v>8</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="22">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="F5" s="25">
+        <v>9</v>
+      </c>
+      <c r="G5" s="7">
+        <v>7</v>
+      </c>
+      <c r="H5" s="6">
+        <v>8</v>
+      </c>
+      <c r="I5" s="22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -744,10 +849,22 @@
       <c r="D6" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="17">
-        <v>4</v>
+      <c r="F6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>9</v>
+      </c>
+      <c r="H6" s="8">
+        <v>10</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="25">
+        <v>12</v>
       </c>
       <c r="B7" s="6">
         <v>11</v>
@@ -755,13 +872,25 @@
       <c r="C7" s="7">
         <v>12</v>
       </c>
-      <c r="D7" s="14">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="17">
-        <v>5</v>
+      <c r="D7" s="22">
+        <v>15</v>
+      </c>
+      <c r="F7" s="25">
+        <v>12</v>
+      </c>
+      <c r="G7" s="6">
+        <v>11</v>
+      </c>
+      <c r="H7" s="7">
+        <v>12</v>
+      </c>
+      <c r="I7" s="22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="25">
+        <v>13</v>
       </c>
       <c r="B8" s="7">
         <v>13</v>
@@ -769,11 +898,23 @@
       <c r="C8" s="6">
         <v>14</v>
       </c>
-      <c r="D8" s="14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="22">
+        <v>14</v>
+      </c>
+      <c r="F8" s="25">
+        <v>13</v>
+      </c>
+      <c r="G8" s="7">
+        <v>13</v>
+      </c>
+      <c r="H8" s="6">
+        <v>14</v>
+      </c>
+      <c r="I8" s="22">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,10 +927,22 @@
       <c r="D9" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="17">
-        <v>0</v>
+      <c r="F9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="8">
+        <v>15</v>
+      </c>
+      <c r="H9" s="8">
+        <v>16</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="26">
+        <v>20</v>
       </c>
       <c r="B10" s="6">
         <v>17</v>
@@ -797,13 +950,25 @@
       <c r="C10" s="7">
         <v>18</v>
       </c>
-      <c r="D10" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="17">
-        <v>1</v>
+      <c r="D10" s="22">
+        <v>17</v>
+      </c>
+      <c r="F10" s="26">
+        <v>26</v>
+      </c>
+      <c r="G10" s="6">
+        <v>17</v>
+      </c>
+      <c r="H10" s="7">
+        <v>18</v>
+      </c>
+      <c r="I10" s="22">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="26">
+        <v>21</v>
       </c>
       <c r="B11" s="7">
         <v>19</v>
@@ -811,11 +976,23 @@
       <c r="C11" s="6">
         <v>20</v>
       </c>
-      <c r="D11" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11" s="22">
+        <v>16</v>
+      </c>
+      <c r="F11" s="26">
+        <v>27</v>
+      </c>
+      <c r="G11" s="7">
+        <v>19</v>
+      </c>
+      <c r="H11" s="6">
+        <v>20</v>
+      </c>
+      <c r="I11" s="22">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -828,10 +1005,22 @@
       <c r="D12" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="17">
-        <v>16</v>
+      <c r="F12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
+        <v>21</v>
+      </c>
+      <c r="H12" s="8">
+        <v>22</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="26">
+        <v>18</v>
       </c>
       <c r="B13" s="6">
         <v>23</v>
@@ -839,13 +1028,25 @@
       <c r="C13" s="7">
         <v>24</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="23">
+        <v>1</v>
+      </c>
+      <c r="F13" s="26">
+        <v>24</v>
+      </c>
+      <c r="G13" s="6">
+        <v>23</v>
+      </c>
+      <c r="H13" s="7">
+        <v>24</v>
+      </c>
+      <c r="I13" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="26">
         <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="17">
-        <v>17</v>
       </c>
       <c r="B14" s="7">
         <v>25</v>
@@ -853,11 +1054,23 @@
       <c r="C14" s="6">
         <v>26</v>
       </c>
-      <c r="D14" s="14">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="D14" s="23">
+        <v>0</v>
+      </c>
+      <c r="F14" s="26">
+        <v>25</v>
+      </c>
+      <c r="G14" s="7">
+        <v>25</v>
+      </c>
+      <c r="H14" s="6">
+        <v>26</v>
+      </c>
+      <c r="I14" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -870,10 +1083,22 @@
       <c r="D15" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="17">
-        <v>20</v>
+      <c r="F15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="8">
+        <v>27</v>
+      </c>
+      <c r="H15" s="8">
+        <v>28</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="24">
+        <v>2</v>
       </c>
       <c r="B16" s="6">
         <v>29</v>
@@ -881,13 +1106,25 @@
       <c r="C16" s="7">
         <v>30</v>
       </c>
-      <c r="D16" s="14">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="17">
-        <v>21</v>
+      <c r="D16" s="23">
+        <v>5</v>
+      </c>
+      <c r="F16" s="24">
+        <v>2</v>
+      </c>
+      <c r="G16" s="6">
+        <v>29</v>
+      </c>
+      <c r="H16" s="7">
+        <v>30</v>
+      </c>
+      <c r="I16" s="23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="24">
+        <v>3</v>
       </c>
       <c r="B17" s="7">
         <v>31</v>
@@ -895,11 +1132,23 @@
       <c r="C17" s="6">
         <v>32</v>
       </c>
-      <c r="D17" s="14">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="D17" s="23">
+        <v>4</v>
+      </c>
+      <c r="F17" s="24">
+        <v>3</v>
+      </c>
+      <c r="G17" s="7">
+        <v>31</v>
+      </c>
+      <c r="H17" s="6">
+        <v>32</v>
+      </c>
+      <c r="I17" s="23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -912,10 +1161,22 @@
       <c r="D18" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="17">
-        <v>24</v>
+      <c r="F18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="8">
+        <v>33</v>
+      </c>
+      <c r="H18" s="8">
+        <v>34</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="24">
+        <v>6</v>
       </c>
       <c r="B19" s="6">
         <v>35</v>
@@ -923,13 +1184,25 @@
       <c r="C19" s="7">
         <v>36</v>
       </c>
-      <c r="D19" s="14">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="17">
-        <v>25</v>
+      <c r="D19" s="27">
+        <v>23</v>
+      </c>
+      <c r="F19" s="24">
+        <v>6</v>
+      </c>
+      <c r="G19" s="6">
+        <v>35</v>
+      </c>
+      <c r="H19" s="7">
+        <v>36</v>
+      </c>
+      <c r="I19" s="27">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="24">
+        <v>7</v>
       </c>
       <c r="B20" s="7">
         <v>37</v>
@@ -937,33 +1210,59 @@
       <c r="C20" s="6">
         <v>38</v>
       </c>
-      <c r="D20" s="14">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="18">
+      <c r="D20" s="27">
+        <v>22</v>
+      </c>
+      <c r="F20" s="24">
+        <v>7</v>
+      </c>
+      <c r="G20" s="7">
+        <v>37</v>
+      </c>
+      <c r="H20" s="6">
+        <v>38</v>
+      </c>
+      <c r="I20" s="27">
         <v>28</v>
       </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="18"/>
       <c r="B21" s="9">
         <v>39</v>
       </c>
       <c r="C21" s="10">
         <v>40</v>
       </c>
-      <c r="D21" s="16">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="D21" s="16"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="9">
+        <v>39</v>
+      </c>
+      <c r="H21" s="10">
+        <v>40</v>
+      </c>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="F22" s="17"/>
+      <c r="I22" s="14"/>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="18"/>
-      <c r="D23" s="16" t="s">
-        <v>2</v>
+      <c r="D23" s="16"/>
+      <c r="F23" s="18"/>
+      <c r="I23" s="16"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="F25" s="28" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
update gpio bit arrangement for 25 bit wide AXI GPIO registers
</commit_message>
<xml_diff>
--- a/design/gpio-bit-arrangement.xlsx
+++ b/design/gpio-bit-arrangement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6440" yWindow="1080" windowWidth="21440" windowHeight="21920" tabRatio="500"/>
+    <workbookView xWindow="9040" yWindow="500" windowWidth="28400" windowHeight="27760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="4">
   <si>
     <t>GND</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>preferred</t>
   </si>
 </sst>
 </file>
@@ -96,7 +93,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,36 +136,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -239,7 +206,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -278,49 +245,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -694,50 +630,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.5" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="15" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="13"/>
+    <col min="4" max="4" width="9.83203125" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:4">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="20"/>
+      <c r="C1" s="15"/>
       <c r="D1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="19" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2">
@@ -746,20 +667,10 @@
       <c r="C2" s="3">
         <v>2</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="F2" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3">
-        <v>2</v>
-      </c>
-      <c r="I2" s="16"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="19" t="s">
+      <c r="D2" s="17"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2">
@@ -768,25 +679,13 @@
       <c r="C3" s="4">
         <v>4</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="5">
         <v>24</v>
       </c>
-      <c r="F3" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="2">
-        <v>3</v>
-      </c>
-      <c r="H3" s="4">
-        <v>4</v>
-      </c>
-      <c r="I3" s="21">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="25">
-        <v>8</v>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>0</v>
       </c>
       <c r="B4" s="6">
         <v>5</v>
@@ -794,25 +693,13 @@
       <c r="C4" s="7">
         <v>6</v>
       </c>
-      <c r="D4" s="22">
-        <v>11</v>
-      </c>
-      <c r="F4" s="25">
-        <v>8</v>
-      </c>
-      <c r="G4" s="6">
-        <v>5</v>
-      </c>
-      <c r="H4" s="7">
-        <v>6</v>
-      </c>
-      <c r="I4" s="22">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="25">
-        <v>9</v>
+      <c r="D4" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>1</v>
       </c>
       <c r="B5" s="7">
         <v>7</v>
@@ -820,23 +707,11 @@
       <c r="C5" s="6">
         <v>8</v>
       </c>
-      <c r="D5" s="22">
-        <v>10</v>
-      </c>
-      <c r="F5" s="25">
-        <v>9</v>
-      </c>
-      <c r="G5" s="7">
-        <v>7</v>
-      </c>
-      <c r="H5" s="6">
-        <v>8</v>
-      </c>
-      <c r="I5" s="22">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -849,22 +724,10 @@
       <c r="D6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="8">
-        <v>9</v>
-      </c>
-      <c r="H6" s="8">
-        <v>10</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="25">
-        <v>12</v>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>4</v>
       </c>
       <c r="B7" s="6">
         <v>11</v>
@@ -872,25 +735,13 @@
       <c r="C7" s="7">
         <v>12</v>
       </c>
-      <c r="D7" s="22">
-        <v>15</v>
-      </c>
-      <c r="F7" s="25">
-        <v>12</v>
-      </c>
-      <c r="G7" s="6">
-        <v>11</v>
-      </c>
-      <c r="H7" s="7">
-        <v>12</v>
-      </c>
-      <c r="I7" s="22">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="25">
-        <v>13</v>
+      <c r="D7" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>5</v>
       </c>
       <c r="B8" s="7">
         <v>13</v>
@@ -898,23 +749,11 @@
       <c r="C8" s="6">
         <v>14</v>
       </c>
-      <c r="D8" s="22">
-        <v>14</v>
-      </c>
-      <c r="F8" s="25">
-        <v>13</v>
-      </c>
-      <c r="G8" s="7">
-        <v>13</v>
-      </c>
-      <c r="H8" s="6">
-        <v>14</v>
-      </c>
-      <c r="I8" s="22">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="D8" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -927,22 +766,10 @@
       <c r="D9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="8">
-        <v>15</v>
-      </c>
-      <c r="H9" s="8">
-        <v>16</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="26">
-        <v>20</v>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>8</v>
       </c>
       <c r="B10" s="6">
         <v>17</v>
@@ -950,25 +777,13 @@
       <c r="C10" s="7">
         <v>18</v>
       </c>
-      <c r="D10" s="22">
-        <v>17</v>
-      </c>
-      <c r="F10" s="26">
-        <v>26</v>
-      </c>
-      <c r="G10" s="6">
-        <v>17</v>
-      </c>
-      <c r="H10" s="7">
-        <v>18</v>
-      </c>
-      <c r="I10" s="22">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="26">
-        <v>21</v>
+      <c r="D10" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>9</v>
       </c>
       <c r="B11" s="7">
         <v>19</v>
@@ -976,23 +791,11 @@
       <c r="C11" s="6">
         <v>20</v>
       </c>
-      <c r="D11" s="22">
-        <v>16</v>
-      </c>
-      <c r="F11" s="26">
-        <v>27</v>
-      </c>
-      <c r="G11" s="7">
-        <v>19</v>
-      </c>
-      <c r="H11" s="6">
-        <v>20</v>
-      </c>
-      <c r="I11" s="22">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="D11" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1005,22 +808,10 @@
       <c r="D12" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="8">
-        <v>21</v>
-      </c>
-      <c r="H12" s="8">
-        <v>22</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="26">
-        <v>18</v>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>12</v>
       </c>
       <c r="B13" s="6">
         <v>23</v>
@@ -1028,25 +819,13 @@
       <c r="C13" s="7">
         <v>24</v>
       </c>
-      <c r="D13" s="23">
-        <v>1</v>
-      </c>
-      <c r="F13" s="26">
-        <v>24</v>
-      </c>
-      <c r="G13" s="6">
-        <v>23</v>
-      </c>
-      <c r="H13" s="7">
-        <v>24</v>
-      </c>
-      <c r="I13" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="26">
-        <v>19</v>
+      <c r="D13" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>13</v>
       </c>
       <c r="B14" s="7">
         <v>25</v>
@@ -1054,23 +833,11 @@
       <c r="C14" s="6">
         <v>26</v>
       </c>
-      <c r="D14" s="23">
-        <v>0</v>
-      </c>
-      <c r="F14" s="26">
-        <v>25</v>
-      </c>
-      <c r="G14" s="7">
-        <v>25</v>
-      </c>
-      <c r="H14" s="6">
-        <v>26</v>
-      </c>
-      <c r="I14" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="D14" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1083,22 +850,10 @@
       <c r="D15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G15" s="8">
-        <v>27</v>
-      </c>
-      <c r="H15" s="8">
-        <v>28</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="24">
-        <v>2</v>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>16</v>
       </c>
       <c r="B16" s="6">
         <v>29</v>
@@ -1106,25 +861,13 @@
       <c r="C16" s="7">
         <v>30</v>
       </c>
-      <c r="D16" s="23">
-        <v>5</v>
-      </c>
-      <c r="F16" s="24">
-        <v>2</v>
-      </c>
-      <c r="G16" s="6">
-        <v>29</v>
-      </c>
-      <c r="H16" s="7">
-        <v>30</v>
-      </c>
-      <c r="I16" s="23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="24">
-        <v>3</v>
+      <c r="D16" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>17</v>
       </c>
       <c r="B17" s="7">
         <v>31</v>
@@ -1132,23 +875,11 @@
       <c r="C17" s="6">
         <v>32</v>
       </c>
-      <c r="D17" s="23">
-        <v>4</v>
-      </c>
-      <c r="F17" s="24">
-        <v>3</v>
-      </c>
-      <c r="G17" s="7">
-        <v>31</v>
-      </c>
-      <c r="H17" s="6">
-        <v>32</v>
-      </c>
-      <c r="I17" s="23">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="D17" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1161,22 +892,10 @@
       <c r="D18" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G18" s="8">
-        <v>33</v>
-      </c>
-      <c r="H18" s="8">
-        <v>34</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="24">
-        <v>6</v>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>20</v>
       </c>
       <c r="B19" s="6">
         <v>35</v>
@@ -1184,25 +903,13 @@
       <c r="C19" s="7">
         <v>36</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="5">
         <v>23</v>
       </c>
-      <c r="F19" s="24">
-        <v>6</v>
-      </c>
-      <c r="G19" s="6">
-        <v>35</v>
-      </c>
-      <c r="H19" s="7">
-        <v>36</v>
-      </c>
-      <c r="I19" s="27">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="24">
-        <v>7</v>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>21</v>
       </c>
       <c r="B20" s="7">
         <v>37</v>
@@ -1210,59 +917,27 @@
       <c r="C20" s="6">
         <v>38</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20" s="5">
         <v>22</v>
       </c>
-      <c r="F20" s="24">
-        <v>7</v>
-      </c>
-      <c r="G20" s="7">
-        <v>37</v>
-      </c>
-      <c r="H20" s="6">
-        <v>38</v>
-      </c>
-      <c r="I20" s="27">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="18"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="16"/>
       <c r="B21" s="9">
         <v>39</v>
       </c>
       <c r="C21" s="10">
         <v>40</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="9">
-        <v>39</v>
-      </c>
-      <c r="H21" s="10">
-        <v>40</v>
-      </c>
-      <c r="I21" s="16"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="F22" s="17"/>
-      <c r="I22" s="14"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="18"/>
-      <c r="D23" s="16"/>
-      <c r="F23" s="18"/>
-      <c r="I23" s="16"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="F25" s="28" t="s">
-        <v>4</v>
-      </c>
+      <c r="D21" s="17"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="16"/>
+      <c r="D23" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>